<commit_message>
modify sql for invline add c.kento=1 in make_balance
</commit_message>
<xml_diff>
--- a/zaikohyo/TFC_kento_2020-01-09.xlsx
+++ b/zaikohyo/TFC_kento_2020-01-09.xlsx
@@ -1360,7 +1360,9 @@
       </c>
       <c r="J8" s="32" t="n"/>
       <c r="K8" s="32" t="inlineStr"/>
-      <c r="L8" s="32" t="inlineStr"/>
+      <c r="L8" s="32" t="n">
+        <v>50</v>
+      </c>
       <c r="M8" s="32" t="inlineStr"/>
       <c r="N8" s="32" t="inlineStr"/>
       <c r="O8" s="28" t="inlineStr"/>

</xml_diff>